<commit_message>
added codon optimization code
</commit_message>
<xml_diff>
--- a/DNA_Sequences/Codon_Optimization/Data/codons_aa.xlsx
+++ b/DNA_Sequences/Codon_Optimization/Data/codons_aa.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">Codon</t>
   </si>
   <si>
+    <t xml:space="preserve">Amino_acid_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amino_acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abreviation_aa</t>
   </si>
   <si>
     <t xml:space="preserve">TTT</t>
@@ -434,12 +434,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,7 +447,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -581,7 +585,7 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -592,7 +596,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,721 +606,721 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>